<commit_message>
test cases login lagout
</commit_message>
<xml_diff>
--- a/TestData/Create_account.xlsx
+++ b/TestData/Create_account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgirish\PycharmProjects\MainAssesment\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370078B1-34C2-4999-B3DF-3FAF2CB77075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D2ED93-0A12-4942-BCD0-99FF6A1019CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FA95EBD7-2971-4A6F-BF5B-3BFFF077D4B7}"/>
   </bookViews>
@@ -50,13 +50,13 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
-    <t>pavan@123</t>
-  </si>
-  <si>
     <t>Pavan</t>
   </si>
   <si>
     <t>pavan111333333@gmail.com</t>
+  </si>
+  <si>
+    <t>pavan@1236</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,23 +456,25 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{62CF2A90-6E6E-424A-9BA7-C6CD9F61B32A}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{FC4F7E0E-DB1E-476C-8913-CF6D17035080}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{831B7974-5B1B-4D29-98CE-967FE22FE70B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added testcases add notes and notepage
</commit_message>
<xml_diff>
--- a/TestData/Create_account.xlsx
+++ b/TestData/Create_account.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgirish\PycharmProjects\MainAssesment\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nampekumar\pycharmProject1\MynotesAssisment\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D2ED93-0A12-4942-BCD0-99FF6A1019CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418F99F3-2AB9-4EAE-B378-3DF0F43CFF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FA95EBD7-2971-4A6F-BF5B-3BFFF077D4B7}"/>
   </bookViews>

</xml_diff>